<commit_message>
Version 1.0.6 Added features file for training Modified readme.md Classifiers updated Deleted unnecessary code Corrections in training code
</commit_message>
<xml_diff>
--- a/results/models/results.xlsx
+++ b/results/models/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="features_1_2sec" sheetId="1" r:id="rId1"/>
@@ -442,9 +442,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
@@ -646,13 +651,13 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="2" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -742,7 +747,7 @@
         <v>0.48</v>
       </c>
       <c r="E4" s="1">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="F4" s="1">
         <v>0.76</v>
@@ -771,7 +776,7 @@
         <v>0.49</v>
       </c>
       <c r="E5" s="1">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="F5" s="1">
         <v>0.78</v>
@@ -800,7 +805,7 @@
         <v>0.93</v>
       </c>
       <c r="E6" s="1">
-        <v>0.82</v>
+        <v>0.73</v>
       </c>
       <c r="F6" s="1">
         <v>0.92</v>
@@ -853,9 +858,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
@@ -1055,11 +1065,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">

</xml_diff>